<commit_message>
able to enter the details from excel and register it to bank
</commit_message>
<xml_diff>
--- a/datafiles/RegistrationData_ParaBank.xlsx
+++ b/datafiles/RegistrationData_ParaBank.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rajiv Deshpande\Documents\ParaBank\ParaBank\datafiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{787A36D9-4617-4097-9834-AA49C541963A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88C020B4-177A-4302-98B8-964AFA857C20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{CC2457E4-5BC9-4E46-999A-1CE45E3E2C1E}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>LastName</t>
   </si>
@@ -75,14 +75,32 @@
     <t>karnataka</t>
   </si>
   <si>
-    <t>sur123</t>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>"580024"</t>
+  </si>
+  <si>
+    <t>"1234567891"</t>
+  </si>
+  <si>
+    <t>"123"</t>
+  </si>
+  <si>
+    <t>"sur123"</t>
+  </si>
+  <si>
+    <t>" Suraj@123"</t>
+  </si>
+  <si>
+    <t>Confirm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -96,6 +114,14 @@
       <color rgb="FF5F7A77"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,14 +141,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -435,10 +464,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CEDB6CC8-16CC-4F78-9F9B-A657CF1574E0}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -449,7 +478,7 @@
     <col min="7" max="7" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -477,8 +506,14 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>19</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -494,21 +529,30 @@
       <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="F2">
-        <v>580024</v>
-      </c>
-      <c r="G2">
-        <v>1234567891</v>
-      </c>
-      <c r="H2">
-        <v>123</v>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" display="Suraj@123" xr:uid="{C3824F13-3B2E-4C31-BC3E-FFE37021990B}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>